<commit_message>
designed data display for VehicleInfo using data in presenter file
</commit_message>
<xml_diff>
--- a/FE_Dashboard/TouchGFX/assets/texts/texts.xlsx
+++ b/FE_Dashboard/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="85">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -198,6 +198,78 @@
   </si>
   <si>
     <t xml:space="preserve">0-9,a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Speed &lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCU Errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Status &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCU Errors &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; Km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt; Km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Status &lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
   </si>
 </sst>
 </file>
@@ -1378,10 +1450,10 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
         <v>60</v>
@@ -1649,22 +1721,174 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>